<commit_message>
work on zonation figure
</commit_message>
<xml_diff>
--- a/src/zia/statistics/lobulus_geometry/plotting/descriptive-stats.xlsx
+++ b/src/zia/statistics/lobulus_geometry/plotting/descriptive-stats.xlsx
@@ -540,13 +540,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.827175823275368</v>
+        <v>1.823608893346713</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2526771870513668</v>
+        <v>0.2477015488992961</v>
       </c>
       <c r="H2" t="n">
-        <v>0.04596759652025957</v>
+        <v>0.04587786065921773</v>
       </c>
       <c r="I2" t="n">
         <v>1.842336779053236</v>
@@ -555,13 +555,13 @@
         <v>0.5332906831698536</v>
       </c>
       <c r="K2" t="n">
-        <v>2.774353943537956</v>
+        <v>2.653413355357386</v>
       </c>
       <c r="L2" t="n">
         <v>1.731584695664099</v>
       </c>
       <c r="M2" t="n">
-        <v>1.961688466834085</v>
+        <v>1.958420803746452</v>
       </c>
       <c r="N2" t="n">
         <v>1580</v>
@@ -592,13 +592,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>5.275970788503913</v>
+        <v>5.276863081535402</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4635215564749451</v>
+        <v>0.4645090419522226</v>
       </c>
       <c r="H3" t="n">
-        <v>0.132731450016605</v>
+        <v>0.1327538980840142</v>
       </c>
       <c r="I3" t="n">
         <v>5.32230492558752</v>
@@ -607,13 +607,13 @@
         <v>2.626385892975756</v>
       </c>
       <c r="K3" t="n">
-        <v>6.586047263249251</v>
+        <v>6.610643094681172</v>
       </c>
       <c r="L3" t="n">
         <v>5.108901737807897</v>
       </c>
       <c r="M3" t="n">
-        <v>5.529475879967699</v>
+        <v>5.530830681375991</v>
       </c>
       <c r="N3" t="n">
         <v>1580</v>
@@ -644,16 +644,16 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.6321661384764302</v>
+        <v>0.6392003561042263</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1034756595570789</v>
+        <v>0.09115656877995283</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01590386519845916</v>
+        <v>0.01608083014820909</v>
       </c>
       <c r="I4" t="n">
-        <v>0.644641396363234</v>
+        <v>0.646184478450162</v>
       </c>
       <c r="J4" t="n">
         <v>0.1339871348603871</v>
@@ -662,10 +662,10 @@
         <v>0.8464523100575919</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5848792988430173</v>
+        <v>0.5914528041362792</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7003863932376948</v>
+        <v>0.701371135587769</v>
       </c>
       <c r="N4" t="n">
         <v>1580</v>
@@ -748,28 +748,28 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1.910845896547076</v>
+        <v>1.896904520907882</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3244547743637403</v>
+        <v>0.3062090223611371</v>
       </c>
       <c r="H6" t="n">
-        <v>0.07415520235744009</v>
+        <v>0.07361417205586859</v>
       </c>
       <c r="I6" t="n">
-        <v>1.939372280213416</v>
+        <v>1.936793500248449</v>
       </c>
       <c r="J6" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K6" t="n">
-        <v>3.029735575675644</v>
+        <v>2.835729222960276</v>
       </c>
       <c r="L6" t="n">
         <v>1.797982365956487</v>
       </c>
       <c r="M6" t="n">
-        <v>2.082558496944985</v>
+        <v>2.067423026826792</v>
       </c>
       <c r="N6" t="n">
         <v>664</v>
@@ -800,13 +800,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.408364357792811</v>
+        <v>5.411277374577539</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5758704759715587</v>
+        <v>0.5796597430553152</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2098852419756142</v>
+        <v>0.2099982889510571</v>
       </c>
       <c r="I7" t="n">
         <v>5.485523774859148</v>
@@ -815,13 +815,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K7" t="n">
-        <v>6.887172561630732</v>
+        <v>6.938669058767234</v>
       </c>
       <c r="L7" t="n">
         <v>5.233840916190425</v>
       </c>
       <c r="M7" t="n">
-        <v>5.746706263803659</v>
+        <v>5.746787744948553</v>
       </c>
       <c r="N7" t="n">
         <v>664</v>
@@ -852,28 +852,28 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.5935821066043051</v>
+        <v>0.621069691072396</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1322070740406806</v>
+        <v>0.1013280337061429</v>
       </c>
       <c r="H8" t="n">
-        <v>0.02303545320454019</v>
+        <v>0.02410217836130549</v>
       </c>
       <c r="I8" t="n">
-        <v>0.6174315944780699</v>
+        <v>0.6318712410716738</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0917208764798314</v>
+        <v>0.2325156717908921</v>
       </c>
       <c r="K8" t="n">
         <v>0.8282910428043042</v>
       </c>
       <c r="L8" t="n">
-        <v>0.5275437319622673</v>
+        <v>0.5683370596860071</v>
       </c>
       <c r="M8" t="n">
-        <v>0.6846325471388102</v>
+        <v>0.6897341251339377</v>
       </c>
       <c r="N8" t="n">
         <v>664</v>
@@ -956,28 +956,28 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2.003845247455911</v>
+        <v>1.992538307358814</v>
       </c>
       <c r="G10" t="n">
-        <v>0.35093115564484</v>
+        <v>0.3422592245503658</v>
       </c>
       <c r="H10" t="n">
-        <v>0.07557645489500918</v>
+        <v>0.07515000557247105</v>
       </c>
       <c r="I10" t="n">
-        <v>2.09491255994804</v>
+        <v>2.088587580457617</v>
       </c>
       <c r="J10" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K10" t="n">
-        <v>2.752654414197818</v>
+        <v>2.650090511426482</v>
       </c>
       <c r="L10" t="n">
-        <v>1.918924035706974</v>
+        <v>1.918660838429597</v>
       </c>
       <c r="M10" t="n">
-        <v>2.217834829923976</v>
+        <v>2.198552332904778</v>
       </c>
       <c r="N10" t="n">
         <v>703</v>
@@ -1008,28 +1008,28 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5.600288572223321</v>
+        <v>5.601702729361006</v>
       </c>
       <c r="G11" t="n">
-        <v>0.6557104192371647</v>
+        <v>0.6566425481665474</v>
       </c>
       <c r="H11" t="n">
-        <v>0.2112188839008555</v>
+        <v>0.2112722198474644</v>
       </c>
       <c r="I11" t="n">
-        <v>5.797527044004138</v>
+        <v>5.79869686149771</v>
       </c>
       <c r="J11" t="n">
         <v>3.103507147695418</v>
       </c>
       <c r="K11" t="n">
-        <v>6.598542428835249</v>
+        <v>6.609786631156294</v>
       </c>
       <c r="L11" t="n">
         <v>5.485821835685517</v>
       </c>
       <c r="M11" t="n">
-        <v>6.003601039683083</v>
+        <v>6.004964101680649</v>
       </c>
       <c r="N11" t="n">
         <v>703</v>
@@ -1060,28 +1060,28 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.5935803779268549</v>
+        <v>0.6198578673323154</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1147206127280737</v>
+        <v>0.09331342184931574</v>
       </c>
       <c r="H12" t="n">
-        <v>0.02238730795998681</v>
+        <v>0.02337838224345617</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6051491848742631</v>
+        <v>0.6261170222036361</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1805755171493738</v>
+        <v>0.2829170448171436</v>
       </c>
       <c r="K12" t="n">
         <v>0.8983534740877451</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5128881361142619</v>
+        <v>0.5595704052670161</v>
       </c>
       <c r="M12" t="n">
-        <v>0.6776313079094067</v>
+        <v>0.6849396903544116</v>
       </c>
       <c r="N12" t="n">
         <v>703</v>
@@ -1164,28 +1164,28 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1.978213641034765</v>
+        <v>1.966719139645023</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4341849979017441</v>
+        <v>0.4233542087602422</v>
       </c>
       <c r="H14" t="n">
-        <v>0.05808235242677077</v>
+        <v>0.05774486224530596</v>
       </c>
       <c r="I14" t="n">
-        <v>2.074001021856211</v>
+        <v>2.068340283453194</v>
       </c>
       <c r="J14" t="n">
         <v>0.5332906831698536</v>
       </c>
       <c r="K14" t="n">
-        <v>3.024717770096984</v>
+        <v>2.983830481778517</v>
       </c>
       <c r="L14" t="n">
         <v>1.811398362884942</v>
       </c>
       <c r="M14" t="n">
-        <v>2.24012966864961</v>
+        <v>2.230389261219646</v>
       </c>
       <c r="N14" t="n">
         <v>1160</v>
@@ -1216,28 +1216,28 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>5.524294853271377</v>
+        <v>5.526001457552354</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7998416197901048</v>
+        <v>0.8010940777128752</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1621988818200982</v>
+        <v>0.1622489894471232</v>
       </c>
       <c r="I15" t="n">
-        <v>5.742495275235555</v>
+        <v>5.745303608859778</v>
       </c>
       <c r="J15" t="n">
         <v>2.626385892975756</v>
       </c>
       <c r="K15" t="n">
-        <v>7.033385671352201</v>
+        <v>7.035320851654557</v>
       </c>
       <c r="L15" t="n">
         <v>5.241019260469624</v>
       </c>
       <c r="M15" t="n">
-        <v>6.051389682243891</v>
+        <v>6.051471102285559</v>
       </c>
       <c r="N15" t="n">
         <v>1160</v>
@@ -1268,28 +1268,28 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.5703009637515482</v>
+        <v>0.5925397291051707</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1392470760588548</v>
+        <v>0.1170967339658341</v>
       </c>
       <c r="H16" t="n">
-        <v>0.01674461285618155</v>
+        <v>0.01739756548981606</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5917152155448135</v>
+        <v>0.6065040924701501</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1135846008642713</v>
+        <v>0.1371178619904701</v>
       </c>
       <c r="K16" t="n">
         <v>0.8573716024224224</v>
       </c>
       <c r="L16" t="n">
-        <v>0.4873570449628974</v>
+        <v>0.5202759370757687</v>
       </c>
       <c r="M16" t="n">
-        <v>0.6704672962147659</v>
+        <v>0.6725491121729937</v>
       </c>
       <c r="N16" t="n">
         <v>1160</v>
@@ -1463,28 +1463,28 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.946683218328497</v>
+        <v>1.933255401280296</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3918738424614589</v>
+        <v>0.3811828278362828</v>
       </c>
       <c r="H2" t="n">
-        <v>0.139763709884318</v>
+        <v>0.1387996488040998</v>
       </c>
       <c r="I2" t="n">
-        <v>2.058061971367709</v>
+        <v>2.048988648905852</v>
       </c>
       <c r="J2" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K2" t="n">
-        <v>2.628631648210432</v>
+        <v>2.551898129832673</v>
       </c>
       <c r="L2" t="n">
         <v>1.865937813590921</v>
       </c>
       <c r="M2" t="n">
-        <v>2.200560835622854</v>
+        <v>2.177917475645361</v>
       </c>
       <c r="N2" t="n">
         <v>194</v>
@@ -1515,28 +1515,28 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2.02705612273965</v>
+        <v>2.01727573658101</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3165585655422127</v>
+        <v>0.3080035363301076</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1498443003347852</v>
+        <v>0.1491213133861236</v>
       </c>
       <c r="I3" t="n">
-        <v>2.103845415700383</v>
+        <v>2.095758641584267</v>
       </c>
       <c r="J3" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K3" t="n">
-        <v>2.508734097145351</v>
+        <v>2.44171032074784</v>
       </c>
       <c r="L3" t="n">
         <v>1.916481815546789</v>
       </c>
       <c r="M3" t="n">
-        <v>2.231280697033813</v>
+        <v>2.222114084534192</v>
       </c>
       <c r="N3" t="n">
         <v>183</v>
@@ -1567,28 +1567,28 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2.056121435627949</v>
+        <v>2.043756139621714</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3082046499486663</v>
+        <v>0.3000608053925014</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1395786179544932</v>
+        <v>0.1387392069658025</v>
       </c>
       <c r="I4" t="n">
-        <v>2.131475391087486</v>
+        <v>2.124355290196353</v>
       </c>
       <c r="J4" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K4" t="n">
-        <v>2.498164998426469</v>
+        <v>2.464758827566032</v>
       </c>
       <c r="L4" t="n">
-        <v>1.980905061664649</v>
+        <v>1.976016985511829</v>
       </c>
       <c r="M4" t="n">
-        <v>2.231280697033813</v>
+        <v>2.203687156632352</v>
       </c>
       <c r="N4" t="n">
         <v>217</v>
@@ -1619,28 +1619,28 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.962541675350053</v>
+        <v>1.95455357919846</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3869675784256106</v>
+        <v>0.38004566116903</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1879774002492236</v>
+        <v>0.1872122794029367</v>
       </c>
       <c r="I5" t="n">
-        <v>2.059288506172639</v>
+        <v>2.052578747001859</v>
       </c>
       <c r="J5" t="n">
         <v>0.7953683386006525</v>
       </c>
       <c r="K5" t="n">
-        <v>2.752654414197818</v>
+        <v>2.650090511426482</v>
       </c>
       <c r="L5" t="n">
         <v>1.918924035706974</v>
       </c>
       <c r="M5" t="n">
-        <v>2.194589017281094</v>
+        <v>2.167650161476405</v>
       </c>
       <c r="N5" t="n">
         <v>109</v>
@@ -1671,28 +1671,28 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.476557651802417</v>
+        <v>5.47824590498048</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7285796328173241</v>
+        <v>0.7297962409385975</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3931939247251947</v>
+        <v>0.393315134239495</v>
       </c>
       <c r="I6" t="n">
-        <v>5.701376431608709</v>
+        <v>5.705203716635312</v>
       </c>
       <c r="J6" t="n">
         <v>3.103507147695418</v>
       </c>
       <c r="K6" t="n">
-        <v>6.598542428835249</v>
+        <v>6.606934632335526</v>
       </c>
       <c r="L6" t="n">
         <v>5.310099655756807</v>
       </c>
       <c r="M6" t="n">
-        <v>5.945959229891914</v>
+        <v>5.950357699336472</v>
       </c>
       <c r="N6" t="n">
         <v>194</v>
@@ -1723,28 +1723,28 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.643010383839449</v>
+        <v>5.644175934709512</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5866587931042349</v>
+        <v>0.5875482287226086</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4171433307951649</v>
+        <v>0.417229490794718</v>
       </c>
       <c r="I7" t="n">
-        <v>5.797527044004138</v>
+        <v>5.79869686149771</v>
       </c>
       <c r="J7" t="n">
         <v>3.103507147695418</v>
       </c>
       <c r="K7" t="n">
-        <v>6.370209114579506</v>
+        <v>6.384692074701062</v>
       </c>
       <c r="L7" t="n">
         <v>5.480331865835714</v>
       </c>
       <c r="M7" t="n">
-        <v>6.022665078251428</v>
+        <v>6.026360924981452</v>
       </c>
       <c r="N7" t="n">
         <v>183</v>
@@ -1775,13 +1775,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.708860873716968</v>
+        <v>5.710436697378626</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5793117819870267</v>
+        <v>0.5800946222405967</v>
       </c>
       <c r="H8" t="n">
-        <v>0.3875427282846927</v>
+        <v>0.3876497021652344</v>
       </c>
       <c r="I8" t="n">
         <v>5.867683280085749</v>
@@ -1790,13 +1790,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K8" t="n">
-        <v>6.451876922855186</v>
+        <v>6.453043684851625</v>
       </c>
       <c r="L8" t="n">
         <v>5.594401606969398</v>
       </c>
       <c r="M8" t="n">
-        <v>6.031561439193745</v>
+        <v>6.032585316639069</v>
       </c>
       <c r="N8" t="n">
         <v>217</v>
@@ -1827,13 +1827,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.532632770496556</v>
+        <v>5.53365462194102</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7238344423926499</v>
+        <v>0.7246658926186493</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5299301094057522</v>
+        <v>0.5300279850230621</v>
       </c>
       <c r="I9" t="n">
         <v>5.751541722556286</v>
@@ -1842,7 +1842,7 @@
         <v>3.325355897311775</v>
       </c>
       <c r="K9" t="n">
-        <v>6.590173720321311</v>
+        <v>6.609786631156294</v>
       </c>
       <c r="L9" t="n">
         <v>5.496789798254783</v>
@@ -1879,28 +1879,28 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.5831466237087514</v>
+        <v>0.6138294384374621</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1241843206563465</v>
+        <v>0.1010747551666274</v>
       </c>
       <c r="H10" t="n">
-        <v>0.04186748761620861</v>
+        <v>0.04407038533259205</v>
       </c>
       <c r="I10" t="n">
-        <v>0.59057841615122</v>
+        <v>0.6143467339513355</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2411205656917387</v>
+        <v>0.33400289002796</v>
       </c>
       <c r="K10" t="n">
         <v>0.8395705979745778</v>
       </c>
       <c r="L10" t="n">
-        <v>0.4957831973461272</v>
+        <v>0.5351844188525889</v>
       </c>
       <c r="M10" t="n">
-        <v>0.6822985972345508</v>
+        <v>0.6896950911171008</v>
       </c>
       <c r="N10" t="n">
         <v>194</v>
@@ -1931,28 +1931,28 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.5874882986029161</v>
+        <v>0.6100584740700076</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1097732217665929</v>
+        <v>0.09093247753469162</v>
       </c>
       <c r="H11" t="n">
-        <v>0.04342838467641872</v>
+        <v>0.04509682005586383</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5955497095456811</v>
+        <v>0.6105696309242599</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2809184928364605</v>
+        <v>0.2829170448171436</v>
       </c>
       <c r="K11" t="n">
         <v>0.8983534740877451</v>
       </c>
       <c r="L11" t="n">
-        <v>0.5061359220562616</v>
+        <v>0.5534981575218157</v>
       </c>
       <c r="M11" t="n">
-        <v>0.6625935963362968</v>
+        <v>0.6681008327662081</v>
       </c>
       <c r="N11" t="n">
         <v>183</v>
@@ -1983,28 +1983,28 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.5980175316049728</v>
+        <v>0.6273929491032257</v>
       </c>
       <c r="G12" t="n">
-        <v>0.110450855330888</v>
+        <v>0.08595202802886791</v>
       </c>
       <c r="H12" t="n">
-        <v>0.04059607527436105</v>
+        <v>0.0425902085513142</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6148824532527171</v>
+        <v>0.6373609610645667</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3177951394689898</v>
+        <v>0.3716583109428941</v>
       </c>
       <c r="K12" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5158132385219121</v>
+        <v>0.5797467277851076</v>
       </c>
       <c r="M12" t="n">
-        <v>0.6790665268480202</v>
+        <v>0.6875397950714414</v>
       </c>
       <c r="N12" t="n">
         <v>217</v>
@@ -2035,28 +2035,28 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.6135449328483342</v>
+        <v>0.6320385226379699</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1105516056378949</v>
+        <v>0.09433206110191901</v>
       </c>
       <c r="H13" t="n">
-        <v>0.05876694638463807</v>
+        <v>0.06053831102549913</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6240876814875089</v>
+        <v>0.6369742851881248</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1805755171493738</v>
+        <v>0.2895920750671321</v>
       </c>
       <c r="K13" t="n">
         <v>0.8323186781348108</v>
       </c>
       <c r="L13" t="n">
-        <v>0.5495402120102101</v>
+        <v>0.5892003147323582</v>
       </c>
       <c r="M13" t="n">
-        <v>0.6858054558323018</v>
+        <v>0.6937957311304603</v>
       </c>
       <c r="N13" t="n">
         <v>109</v>
@@ -2386,28 +2386,28 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.964678375653258</v>
+        <v>1.949467041766575</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3296830916695338</v>
+        <v>0.3149086628899231</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2082554913086793</v>
+        <v>0.206643093141484</v>
       </c>
       <c r="I2" t="n">
-        <v>2.014755028578931</v>
+        <v>2.009808855260363</v>
       </c>
       <c r="J2" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K2" t="n">
-        <v>2.662859452006266</v>
+        <v>2.518546032551106</v>
       </c>
       <c r="L2" t="n">
         <v>1.848973323424587</v>
       </c>
       <c r="M2" t="n">
-        <v>2.12421948725473</v>
+        <v>2.122769611315021</v>
       </c>
       <c r="N2" t="n">
         <v>89</v>
@@ -2438,13 +2438,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.866618157513416</v>
+        <v>1.850996109965676</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3467273084476595</v>
+        <v>0.3252596706564639</v>
       </c>
       <c r="H3" t="n">
-        <v>0.195674751047112</v>
+        <v>0.1940371154908274</v>
       </c>
       <c r="I3" t="n">
         <v>1.897465232829924</v>
@@ -2453,13 +2453,13 @@
         <v>0.8343206788338349</v>
       </c>
       <c r="K3" t="n">
-        <v>3.029735575675644</v>
+        <v>2.835729222960276</v>
       </c>
       <c r="L3" t="n">
         <v>1.74701711047923</v>
       </c>
       <c r="M3" t="n">
-        <v>2.058330729602883</v>
+        <v>2.042593971272582</v>
       </c>
       <c r="N3" t="n">
         <v>91</v>
@@ -2490,22 +2490,22 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.878511825581916</v>
+        <v>1.858491062097516</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3717467226275195</v>
+        <v>0.3422495795814258</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2049624436809242</v>
+        <v>0.2027779992966844</v>
       </c>
       <c r="I4" t="n">
-        <v>1.890924709589787</v>
+        <v>1.882023802221668</v>
       </c>
       <c r="J4" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K4" t="n">
-        <v>2.915475937024081</v>
+        <v>2.672606976251537</v>
       </c>
       <c r="L4" t="n">
         <v>1.757623611114369</v>
@@ -2542,28 +2542,28 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.900963584741721</v>
+        <v>1.88724066108023</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3422724205654411</v>
+        <v>0.3244188949039107</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1673705111077855</v>
+        <v>0.1661622750502658</v>
       </c>
       <c r="I5" t="n">
-        <v>1.934201036966176</v>
+        <v>1.931741768443048</v>
       </c>
       <c r="J5" t="n">
         <v>0.8700650914891171</v>
       </c>
       <c r="K5" t="n">
-        <v>2.910060212050245</v>
+        <v>2.766268652690087</v>
       </c>
       <c r="L5" t="n">
         <v>1.786131459996834</v>
       </c>
       <c r="M5" t="n">
-        <v>2.095613594017423</v>
+        <v>2.092863119131768</v>
       </c>
       <c r="N5" t="n">
         <v>129</v>
@@ -2594,13 +2594,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1.980539964385784</v>
+        <v>1.964282928487492</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2327965956806541</v>
+        <v>0.2058158581173092</v>
       </c>
       <c r="H6" t="n">
-        <v>0.190577546929824</v>
+        <v>0.18901321292114</v>
       </c>
       <c r="I6" t="n">
         <v>1.953128267604442</v>
@@ -2609,13 +2609,13 @@
         <v>1.399172831561925</v>
       </c>
       <c r="K6" t="n">
-        <v>2.70826646939756</v>
+        <v>2.556311117416005</v>
       </c>
       <c r="L6" t="n">
         <v>1.845446522957879</v>
       </c>
       <c r="M6" t="n">
-        <v>2.081466061814404</v>
+        <v>2.078746921885097</v>
       </c>
       <c r="N6" t="n">
         <v>108</v>
@@ -2646,22 +2646,22 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1.884450525191225</v>
+        <v>1.876635204825408</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3087484709598031</v>
+        <v>0.3001432810207037</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1476015566341322</v>
+        <v>0.1469894134994792</v>
       </c>
       <c r="I7" t="n">
-        <v>1.943489519379807</v>
+        <v>1.942992090009003</v>
       </c>
       <c r="J7" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K7" t="n">
-        <v>2.507753195519157</v>
+        <v>2.377613177299331</v>
       </c>
       <c r="L7" t="n">
         <v>1.794527668581623</v>
@@ -2698,13 +2698,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.512613377371489</v>
+        <v>5.515070328431229</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6030912576102199</v>
+        <v>0.6054412021314753</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5843358493308478</v>
+        <v>0.5845962856223083</v>
       </c>
       <c r="I8" t="n">
         <v>5.645502183422829</v>
@@ -2713,13 +2713,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K8" t="n">
-        <v>6.452525510911671</v>
+        <v>6.48142020965164</v>
       </c>
       <c r="L8" t="n">
         <v>5.374573919981956</v>
       </c>
       <c r="M8" t="n">
-        <v>5.850918955581841</v>
+        <v>5.86392963111863</v>
       </c>
       <c r="N8" t="n">
         <v>89</v>
@@ -2750,13 +2750,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.321347203364377</v>
+        <v>5.324051834839823</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6152640835248844</v>
+        <v>0.6189843483771933</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5578287584219462</v>
+        <v>0.5581122808384094</v>
       </c>
       <c r="I9" t="n">
         <v>5.402360224105125</v>
@@ -2765,13 +2765,13 @@
         <v>3.404537143359399</v>
       </c>
       <c r="K9" t="n">
-        <v>6.887172561630732</v>
+        <v>6.938669058767234</v>
       </c>
       <c r="L9" t="n">
         <v>5.161678167289589</v>
       </c>
       <c r="M9" t="n">
-        <v>5.72155468403585</v>
+        <v>5.725540649136007</v>
       </c>
       <c r="N9" t="n">
         <v>91</v>
@@ -2802,13 +2802,13 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5.327099350756062</v>
+        <v>5.333902541733471</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6314100183216638</v>
+        <v>0.6409332494744789</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5812341906997563</v>
+        <v>0.5819764796907376</v>
       </c>
       <c r="I10" t="n">
         <v>5.420859952388762</v>
@@ -2817,13 +2817,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K10" t="n">
-        <v>6.621626094838571</v>
+        <v>6.751118290695786</v>
       </c>
       <c r="L10" t="n">
         <v>5.172880687777769</v>
       </c>
       <c r="M10" t="n">
-        <v>5.655948738430183</v>
+        <v>5.656147773537207</v>
       </c>
       <c r="N10" t="n">
         <v>84</v>
@@ -2854,13 +2854,13 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5.385623355175486</v>
+        <v>5.388663590755486</v>
       </c>
       <c r="G11" t="n">
-        <v>0.6009108479689694</v>
+        <v>0.6051070100552213</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4741776964192704</v>
+        <v>0.4744453742364558</v>
       </c>
       <c r="I11" t="n">
         <v>5.489708753096211</v>
@@ -2869,7 +2869,7 @@
         <v>3.471483932990012</v>
       </c>
       <c r="K11" t="n">
-        <v>6.744815970097845</v>
+        <v>6.817137672895941</v>
       </c>
       <c r="L11" t="n">
         <v>5.202727243181549</v>
@@ -2906,13 +2906,13 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>5.538950347674866</v>
+        <v>5.541943194508104</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3671783774397002</v>
+        <v>0.3722691767716104</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5329857457096758</v>
+        <v>0.5332737325304781</v>
       </c>
       <c r="I12" t="n">
         <v>5.508287005013052</v>
@@ -2921,7 +2921,7 @@
         <v>4.425726442429338</v>
       </c>
       <c r="K12" t="n">
-        <v>6.446455927288081</v>
+        <v>6.487980037619621</v>
       </c>
       <c r="L12" t="n">
         <v>5.342389236610555</v>
@@ -2958,13 +2958,13 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5.373376390504132</v>
+        <v>5.374496434348087</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5778717451026887</v>
+        <v>0.5789011602909603</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4208753209580932</v>
+        <v>0.4209630495626155</v>
       </c>
       <c r="I13" t="n">
         <v>5.486124459172903</v>
@@ -2973,7 +2973,7 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K13" t="n">
-        <v>6.306267835088618</v>
+        <v>6.325182144766187</v>
       </c>
       <c r="L13" t="n">
         <v>5.193372385900524</v>
@@ -3010,28 +3010,28 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.5868990318738765</v>
+        <v>0.6205717047745558</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1289064155052375</v>
+        <v>0.1028023742003257</v>
       </c>
       <c r="H14" t="n">
-        <v>0.06221117295640942</v>
+        <v>0.06578046914529619</v>
       </c>
       <c r="I14" t="n">
-        <v>0.6029607922242649</v>
+        <v>0.6389413665911835</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1685812617723295</v>
+        <v>0.2325156717908921</v>
       </c>
       <c r="K14" t="n">
         <v>0.789338744286178</v>
       </c>
       <c r="L14" t="n">
-        <v>0.5322613457473647</v>
+        <v>0.5693841919990569</v>
       </c>
       <c r="M14" t="n">
-        <v>0.6751292203552718</v>
+        <v>0.6814540912689894</v>
       </c>
       <c r="N14" t="n">
         <v>89</v>
@@ -3062,28 +3062,28 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.5946302196490982</v>
+        <v>0.6263714654792422</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1292500546907334</v>
+        <v>0.09334324911092787</v>
       </c>
       <c r="H15" t="n">
-        <v>0.06233418427147733</v>
+        <v>0.06566157094171761</v>
       </c>
       <c r="I15" t="n">
-        <v>0.6172363636367152</v>
+        <v>0.624454499627617</v>
       </c>
       <c r="J15" t="n">
-        <v>0.09988387573118765</v>
+        <v>0.2440664538245969</v>
       </c>
       <c r="K15" t="n">
         <v>0.8282910428043042</v>
       </c>
       <c r="L15" t="n">
-        <v>0.5408798453728703</v>
+        <v>0.5748984431859578</v>
       </c>
       <c r="M15" t="n">
-        <v>0.6790195757636523</v>
+        <v>0.681866084176064</v>
       </c>
       <c r="N15" t="n">
         <v>91</v>
@@ -3114,25 +3114,25 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.5851302936958452</v>
+        <v>0.6170181544443787</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1571151077693828</v>
+        <v>0.1106824392401934</v>
       </c>
       <c r="H16" t="n">
-        <v>0.06384294910173698</v>
+        <v>0.06732219995007901</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6206212617296498</v>
+        <v>0.6307470615337923</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0917208764798314</v>
+        <v>0.2806765422822406</v>
       </c>
       <c r="K16" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5341009822185109</v>
+        <v>0.5518949251423089</v>
       </c>
       <c r="M16" t="n">
         <v>0.6988738601695477</v>
@@ -3166,28 +3166,28 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.5907927325673585</v>
+        <v>0.6175478370957609</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1360386631658067</v>
+        <v>0.1079640449895387</v>
       </c>
       <c r="H17" t="n">
-        <v>0.05201639968395227</v>
+        <v>0.05437205528703914</v>
       </c>
       <c r="I17" t="n">
-        <v>0.6270085070524034</v>
+        <v>0.6395761291343045</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1248790313520531</v>
+        <v>0.2421434021949473</v>
       </c>
       <c r="K17" t="n">
         <v>0.82199317727846</v>
       </c>
       <c r="L17" t="n">
-        <v>0.4906886086151637</v>
+        <v>0.546756242986877</v>
       </c>
       <c r="M17" t="n">
-        <v>0.6935988984456756</v>
+        <v>0.6951584872370929</v>
       </c>
       <c r="N17" t="n">
         <v>129</v>
@@ -3218,28 +3218,28 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.5829377335537662</v>
+        <v>0.6141984876982431</v>
       </c>
       <c r="G18" t="n">
-        <v>0.131013225236593</v>
+        <v>0.09416803627240024</v>
       </c>
       <c r="H18" t="n">
-        <v>0.05609320956467621</v>
+        <v>0.05910127703474029</v>
       </c>
       <c r="I18" t="n">
-        <v>0.6089594376519225</v>
+        <v>0.6301779477278668</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1421651928079205</v>
+        <v>0.2862226394628783</v>
       </c>
       <c r="K18" t="n">
         <v>0.7712131631523208</v>
       </c>
       <c r="L18" t="n">
-        <v>0.5288444517443309</v>
+        <v>0.5717656351114314</v>
       </c>
       <c r="M18" t="n">
-        <v>0.6761903872236612</v>
+        <v>0.6822046196577445</v>
       </c>
       <c r="N18" t="n">
         <v>108</v>
@@ -3270,28 +3270,28 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.6102617948771083</v>
+        <v>0.6278095531192219</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1167934249425289</v>
+        <v>0.09831722481253441</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04779939280659024</v>
+        <v>0.04917383930829002</v>
       </c>
       <c r="I19" t="n">
-        <v>0.6232995888620058</v>
+        <v>0.632543795663103</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2755400212510998</v>
+        <v>0.3117164228163452</v>
       </c>
       <c r="K19" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L19" t="n">
-        <v>0.5431490953892137</v>
+        <v>0.5769392799030744</v>
       </c>
       <c r="M19" t="n">
-        <v>0.6863557281621471</v>
+        <v>0.6914108707608204</v>
       </c>
       <c r="N19" t="n">
         <v>163</v>
@@ -3725,28 +3725,28 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2.027675124321077</v>
+        <v>2.01989806326531</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3779422925790901</v>
+        <v>0.369774652088004</v>
       </c>
       <c r="H2" t="n">
-        <v>0.152841763275233</v>
+        <v>0.1522555452412861</v>
       </c>
       <c r="I2" t="n">
-        <v>2.083368573040024</v>
+        <v>2.07514361230909</v>
       </c>
       <c r="J2" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K2" t="n">
-        <v>2.968669263719774</v>
+        <v>2.941397947026892</v>
       </c>
       <c r="L2" t="n">
         <v>1.919993162947441</v>
       </c>
       <c r="M2" t="n">
-        <v>2.229559309431631</v>
+        <v>2.227347323560678</v>
       </c>
       <c r="N2" t="n">
         <v>176</v>
@@ -3777,28 +3777,28 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2.053359157075526</v>
+        <v>2.041590451602869</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3429307662081154</v>
+        <v>0.333244864647125</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1608315017357869</v>
+        <v>0.159909705581358</v>
       </c>
       <c r="I3" t="n">
-        <v>2.126587941180949</v>
+        <v>2.123891454831814</v>
       </c>
       <c r="J3" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K3" t="n">
-        <v>2.678147594724294</v>
+        <v>2.588905613370616</v>
       </c>
       <c r="L3" t="n">
         <v>2.002189559042013</v>
       </c>
       <c r="M3" t="n">
-        <v>2.230170028926601</v>
+        <v>2.221658445156922</v>
       </c>
       <c r="N3" t="n">
         <v>163</v>
@@ -3829,28 +3829,28 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.97504422575791</v>
+        <v>1.968190091274026</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4290832181548727</v>
+        <v>0.4223687353962265</v>
       </c>
       <c r="H4" t="n">
-        <v>0.166328728891336</v>
+        <v>0.1657515066390508</v>
       </c>
       <c r="I4" t="n">
-        <v>2.099820850827959</v>
+        <v>2.08787510344284</v>
       </c>
       <c r="J4" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K4" t="n">
-        <v>2.844577487805271</v>
+        <v>2.768069920718018</v>
       </c>
       <c r="L4" t="n">
-        <v>1.822068496201865</v>
+        <v>1.818882086110199</v>
       </c>
       <c r="M4" t="n">
-        <v>2.227142571037542</v>
+        <v>2.217889961659767</v>
       </c>
       <c r="N4" t="n">
         <v>141</v>
@@ -3881,28 +3881,28 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.93266277731144</v>
+        <v>1.914816770225321</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5787202625915574</v>
+        <v>0.561352785528257</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1701614693905654</v>
+        <v>0.1685902160792388</v>
       </c>
       <c r="I5" t="n">
-        <v>2.042117612882165</v>
+        <v>2.031636052427815</v>
       </c>
       <c r="J5" t="n">
         <v>0.5332906831698536</v>
       </c>
       <c r="K5" t="n">
-        <v>2.893605221879439</v>
+        <v>2.852029592384894</v>
       </c>
       <c r="L5" t="n">
         <v>1.635616462164843</v>
       </c>
       <c r="M5" t="n">
-        <v>2.376621454665375</v>
+        <v>2.365643818331526</v>
       </c>
       <c r="N5" t="n">
         <v>129</v>
@@ -3933,28 +3933,28 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1.947606697962776</v>
+        <v>1.935111905833545</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4409839182127118</v>
+        <v>0.4298437062749274</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09862089873113658</v>
+        <v>0.09798820033749661</v>
       </c>
       <c r="I6" t="n">
-        <v>2.062761037821935</v>
+        <v>2.058604440228247</v>
       </c>
       <c r="J6" t="n">
         <v>0.7335353824154486</v>
       </c>
       <c r="K6" t="n">
-        <v>3.024717770096984</v>
+        <v>2.983830481778517</v>
       </c>
       <c r="L6" t="n">
         <v>1.728311280862017</v>
       </c>
       <c r="M6" t="n">
-        <v>2.248141259485571</v>
+        <v>2.235675196854505</v>
       </c>
       <c r="N6" t="n">
         <v>390</v>
@@ -3985,28 +3985,28 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1.961478961527845</v>
+        <v>1.94964652011477</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4120361432353322</v>
+        <v>0.3993830540212935</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1545861981199159</v>
+        <v>0.1536536710990301</v>
       </c>
       <c r="I7" t="n">
-        <v>2.040200629003406</v>
+        <v>2.039802548737248</v>
       </c>
       <c r="J7" t="n">
         <v>0.7953683386006525</v>
       </c>
       <c r="K7" t="n">
-        <v>2.715148701548735</v>
+        <v>2.64351783272584</v>
       </c>
       <c r="L7" t="n">
         <v>1.758258510508658</v>
       </c>
       <c r="M7" t="n">
-        <v>2.234512170516562</v>
+        <v>2.220325863822588</v>
       </c>
       <c r="N7" t="n">
         <v>161</v>
@@ -4037,13 +4037,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.635987905730309</v>
+        <v>5.637085069515622</v>
       </c>
       <c r="G8" t="n">
-        <v>0.693978318147591</v>
+        <v>0.6949056986685912</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4248285728701899</v>
+        <v>0.4249112747022229</v>
       </c>
       <c r="I8" t="n">
         <v>5.764685719754578</v>
@@ -4052,13 +4052,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K8" t="n">
-        <v>6.858084803740149</v>
+        <v>6.861130893603807</v>
       </c>
       <c r="L8" t="n">
         <v>5.482352665481649</v>
       </c>
       <c r="M8" t="n">
-        <v>6.030989507277965</v>
+        <v>6.031577755886696</v>
       </c>
       <c r="N8" t="n">
         <v>176</v>
@@ -4089,22 +4089,22 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.680404641341724</v>
+        <v>5.681806326782803</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6415972647037259</v>
+        <v>0.642495381380062</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4449236295491</v>
+        <v>0.4450334180260322</v>
       </c>
       <c r="I9" t="n">
-        <v>5.846493981015811</v>
+        <v>5.851436589113804</v>
       </c>
       <c r="J9" t="n">
         <v>3.103507147695418</v>
       </c>
       <c r="K9" t="n">
-        <v>6.6252552568581</v>
+        <v>6.629975660164896</v>
       </c>
       <c r="L9" t="n">
         <v>5.624381083557052</v>
@@ -4141,13 +4141,13 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5.539376229831118</v>
+        <v>5.540188149212362</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8005031501112283</v>
+        <v>0.8011552122196162</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4664996333462487</v>
+        <v>0.4665680092929153</v>
       </c>
       <c r="I10" t="n">
         <v>5.791926969698129</v>
@@ -4156,7 +4156,7 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K10" t="n">
-        <v>6.910906860454904</v>
+        <v>6.925566203721102</v>
       </c>
       <c r="L10" t="n">
         <v>5.247562174750791</v>
@@ -4193,22 +4193,22 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5.42311954940064</v>
+        <v>5.425841460475396</v>
       </c>
       <c r="G11" t="n">
-        <v>1.068253013467692</v>
+        <v>1.070641499672923</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4774790522382003</v>
+        <v>0.4777187031454709</v>
       </c>
       <c r="I11" t="n">
-        <v>5.696423759583511</v>
+        <v>5.698635790589271</v>
       </c>
       <c r="J11" t="n">
         <v>2.626385892975756</v>
       </c>
       <c r="K11" t="n">
-        <v>7.033385671352201</v>
+        <v>7.035320851654557</v>
       </c>
       <c r="L11" t="n">
         <v>4.827783017296207</v>
@@ -4245,13 +4245,13 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>5.452928027250154</v>
+        <v>5.455041030763025</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8044747374713572</v>
+        <v>0.8058470285001765</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2761197439535054</v>
+        <v>0.2762267400455189</v>
       </c>
       <c r="I12" t="n">
         <v>5.679464166400967</v>
@@ -4260,13 +4260,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K12" t="n">
-        <v>6.932961021072205</v>
+        <v>6.936079922541598</v>
       </c>
       <c r="L12" t="n">
         <v>5.069646770592492</v>
       </c>
       <c r="M12" t="n">
-        <v>6.054966090858604</v>
+        <v>6.060032807614627</v>
       </c>
       <c r="N12" t="n">
         <v>390</v>
@@ -4297,13 +4297,13 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5.484880751187162</v>
+        <v>5.486547874674134</v>
       </c>
       <c r="G13" t="n">
-        <v>0.7498409949617413</v>
+        <v>0.7512257146246594</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4322691596991138</v>
+        <v>0.4324005474359706</v>
       </c>
       <c r="I13" t="n">
         <v>5.675603915645937</v>
@@ -4312,13 +4312,13 @@
         <v>3.325355897311775</v>
       </c>
       <c r="K13" t="n">
-        <v>6.707517080107649</v>
+        <v>6.709816841136266</v>
       </c>
       <c r="L13" t="n">
         <v>5.096207908953919</v>
       </c>
       <c r="M13" t="n">
-        <v>5.969597483155503</v>
+        <v>5.97156350951846</v>
       </c>
       <c r="N13" t="n">
         <v>161</v>
@@ -4349,25 +4349,25 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.5857709193048275</v>
+        <v>0.6003347683706112</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1329728165385802</v>
+        <v>0.1160309076050706</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0441541443735378</v>
+        <v>0.04525193580205081</v>
       </c>
       <c r="I14" t="n">
-        <v>0.6102639310533111</v>
+        <v>0.6202845713234406</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1237485878431483</v>
+        <v>0.140308145699986</v>
       </c>
       <c r="K14" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L14" t="n">
-        <v>0.5257852015146978</v>
+        <v>0.5424733341567819</v>
       </c>
       <c r="M14" t="n">
         <v>0.6761759592426906</v>
@@ -4401,28 +4401,28 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.5723669036143473</v>
+        <v>0.5976113680796392</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1242973708214847</v>
+        <v>0.1031309143667258</v>
       </c>
       <c r="H15" t="n">
-        <v>0.04483123584831875</v>
+        <v>0.0468085349079977</v>
       </c>
       <c r="I15" t="n">
-        <v>0.5953969461266823</v>
+        <v>0.6172803842404637</v>
       </c>
       <c r="J15" t="n">
-        <v>0.2162620647147831</v>
+        <v>0.264455620232835</v>
       </c>
       <c r="K15" t="n">
         <v>0.8001063651376856</v>
       </c>
       <c r="L15" t="n">
-        <v>0.4815319869352283</v>
+        <v>0.5316415687408671</v>
       </c>
       <c r="M15" t="n">
-        <v>0.6689834004650217</v>
+        <v>0.672239613859032</v>
       </c>
       <c r="N15" t="n">
         <v>163</v>
@@ -4453,28 +4453,28 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.5921420745872161</v>
+        <v>0.6066075046175853</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1235346827580389</v>
+        <v>0.1093643764095957</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0498673585657938</v>
+        <v>0.05108556753470667</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6061648047024184</v>
+        <v>0.6167779471045608</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2047304860267609</v>
+        <v>0.2371630172537319</v>
       </c>
       <c r="K16" t="n">
         <v>0.8214599846910372</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5220841771130588</v>
+        <v>0.5525133908091606</v>
       </c>
       <c r="M16" t="n">
-        <v>0.6700121568387776</v>
+        <v>0.6770166903164951</v>
       </c>
       <c r="N16" t="n">
         <v>141</v>
@@ -4505,28 +4505,28 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.5622375150939701</v>
+        <v>0.5951636545536438</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1547965233184512</v>
+        <v>0.1187858980220158</v>
       </c>
       <c r="H17" t="n">
-        <v>0.04950225297347526</v>
+        <v>0.05240123790638262</v>
       </c>
       <c r="I17" t="n">
-        <v>0.5938296269051558</v>
+        <v>0.6018539153374356</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1646285393981005</v>
+        <v>0.3170446740347905</v>
       </c>
       <c r="K17" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L17" t="n">
-        <v>0.4535882707391392</v>
+        <v>0.5209241413025247</v>
       </c>
       <c r="M17" t="n">
-        <v>0.670475405576059</v>
+        <v>0.672009891820827</v>
       </c>
       <c r="N17" t="n">
         <v>129</v>
@@ -4557,28 +4557,28 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.5597047242657358</v>
+        <v>0.5833627819088471</v>
       </c>
       <c r="G18" t="n">
-        <v>0.144517774413103</v>
+        <v>0.1224112164859319</v>
       </c>
       <c r="H18" t="n">
-        <v>0.02834175041033097</v>
+        <v>0.02953972272652664</v>
       </c>
       <c r="I18" t="n">
-        <v>0.5719351790148075</v>
+        <v>0.5899470192179559</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1135846008642713</v>
+        <v>0.1371178619904701</v>
       </c>
       <c r="K18" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L18" t="n">
-        <v>0.4778018257228838</v>
+        <v>0.5055544048802105</v>
       </c>
       <c r="M18" t="n">
-        <v>0.6702097190386882</v>
+        <v>0.6715451256098958</v>
       </c>
       <c r="N18" t="n">
         <v>390</v>
@@ -4609,28 +4609,28 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.5642988598599444</v>
+        <v>0.5866910496822315</v>
       </c>
       <c r="G19" t="n">
-        <v>0.143288113808251</v>
+        <v>0.1213202418942717</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04447298036844821</v>
+        <v>0.04623773215019079</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5911659968088238</v>
+        <v>0.6121822507528796</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1513304638285367</v>
+        <v>0.211796839315088</v>
       </c>
       <c r="K19" t="n">
         <v>0.8573716024224224</v>
       </c>
       <c r="L19" t="n">
-        <v>0.4772253033069047</v>
+        <v>0.5029938974006266</v>
       </c>
       <c r="M19" t="n">
-        <v>0.6681829984352</v>
+        <v>0.6708228415992527</v>
       </c>
       <c r="N19" t="n">
         <v>161</v>
@@ -5064,13 +5064,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.811434676685927</v>
+        <v>1.808581694180754</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2918877867150161</v>
+        <v>0.2874530187777741</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1009473078820546</v>
+        <v>0.1007883173829554</v>
       </c>
       <c r="I2" t="n">
         <v>1.844157881901027</v>
@@ -5079,13 +5079,13 @@
         <v>0.5332906831698536</v>
       </c>
       <c r="K2" t="n">
-        <v>2.774353943537956</v>
+        <v>2.653413355357386</v>
       </c>
       <c r="L2" t="n">
         <v>1.730976765006845</v>
       </c>
       <c r="M2" t="n">
-        <v>1.977474049731606</v>
+        <v>1.974342277246353</v>
       </c>
       <c r="N2" t="n">
         <v>322</v>
@@ -5116,13 +5116,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.803437477242384</v>
+        <v>1.7986534195647</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2312047819576145</v>
+        <v>0.2258057772646862</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09897649006359216</v>
+        <v>0.09871393078822267</v>
       </c>
       <c r="I3" t="n">
         <v>1.820943141803164</v>
@@ -5131,13 +5131,13 @@
         <v>0.7335353824154486</v>
       </c>
       <c r="K3" t="n">
-        <v>2.352092404829444</v>
+        <v>2.263055439520928</v>
       </c>
       <c r="L3" t="n">
-        <v>1.735105572440935</v>
+        <v>1.731382052111681</v>
       </c>
       <c r="M3" t="n">
-        <v>1.923733460739929</v>
+        <v>1.918126094959436</v>
       </c>
       <c r="N3" t="n">
         <v>332</v>
@@ -5168,13 +5168,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.844746694965231</v>
+        <v>1.842164492405197</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2204325816813731</v>
+        <v>0.2153864253389289</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1137519542904054</v>
+        <v>0.113592728859413</v>
       </c>
       <c r="I4" t="n">
         <v>1.853173021481741</v>
@@ -5183,13 +5183,13 @@
         <v>0.8700650914891171</v>
       </c>
       <c r="K4" t="n">
-        <v>2.774310952382516</v>
+        <v>2.616753228591421</v>
       </c>
       <c r="L4" t="n">
         <v>1.734907290224331</v>
       </c>
       <c r="M4" t="n">
-        <v>1.970506429049383</v>
+        <v>1.964455262285619</v>
       </c>
       <c r="N4" t="n">
         <v>263</v>
@@ -5220,13 +5220,13 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.836943790527726</v>
+        <v>1.832678765806504</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2385260739560755</v>
+        <v>0.2314990101819192</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1188220160762656</v>
+        <v>0.1185461345612166</v>
       </c>
       <c r="I5" t="n">
         <v>1.845978984748819</v>
@@ -5241,7 +5241,7 @@
         <v>1.741481479814763</v>
       </c>
       <c r="M5" t="n">
-        <v>1.953588132906543</v>
+        <v>1.946122490723221</v>
       </c>
       <c r="N5" t="n">
         <v>239</v>
@@ -5272,13 +5272,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1.811652417872037</v>
+        <v>1.806631902987686</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2524617698827712</v>
+        <v>0.2452887686647225</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1108713274380313</v>
+        <v>0.110564076916817</v>
       </c>
       <c r="I6" t="n">
         <v>1.837133213530358</v>
@@ -5287,13 +5287,13 @@
         <v>0.7335353824154486</v>
       </c>
       <c r="K6" t="n">
-        <v>2.454990292960388</v>
+        <v>2.378936282253052</v>
       </c>
       <c r="L6" t="n">
         <v>1.707314507576331</v>
       </c>
       <c r="M6" t="n">
-        <v>1.938262737486421</v>
+        <v>1.935573634976695</v>
       </c>
       <c r="N6" t="n">
         <v>267</v>
@@ -5324,13 +5324,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1.891754459579144</v>
+        <v>1.891182204064268</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2672131117134728</v>
+        <v>0.266500056982511</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1509784422823249</v>
+        <v>0.1509327713202262</v>
       </c>
       <c r="I7" t="n">
         <v>1.891534641922197</v>
@@ -5376,13 +5376,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.246950264694122</v>
+        <v>5.247641536265799</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5451626140071784</v>
+        <v>0.5460353002057146</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2924011064980515</v>
+        <v>0.2924396295566383</v>
       </c>
       <c r="I8" t="n">
         <v>5.341969634498135</v>
@@ -5391,7 +5391,7 @@
         <v>2.626385892975756</v>
       </c>
       <c r="K8" t="n">
-        <v>6.571213889318972</v>
+        <v>6.58652356783955</v>
       </c>
       <c r="L8" t="n">
         <v>5.10023354364358</v>
@@ -5428,13 +5428,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.227961540435168</v>
+        <v>5.229293788007805</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4258131433223984</v>
+        <v>0.4270859564476012</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2869216648702139</v>
+        <v>0.2869947814546807</v>
       </c>
       <c r="I9" t="n">
         <v>5.277178661540797</v>
@@ -5449,7 +5449,7 @@
         <v>5.10314463109661</v>
       </c>
       <c r="M9" t="n">
-        <v>5.473958552117868</v>
+        <v>5.474112666580189</v>
       </c>
       <c r="N9" t="n">
         <v>332</v>
@@ -5480,13 +5480,13 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5.314410837664624</v>
+        <v>5.315071285749745</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3976461319381989</v>
+        <v>0.3985307431043084</v>
       </c>
       <c r="H10" t="n">
-        <v>0.327700610786488</v>
+        <v>0.3277413357600548</v>
       </c>
       <c r="I10" t="n">
         <v>5.327953878031683</v>
@@ -5495,7 +5495,7 @@
         <v>3.471483932990012</v>
       </c>
       <c r="K10" t="n">
-        <v>6.586047263249251</v>
+        <v>6.610643094681172</v>
       </c>
       <c r="L10" t="n">
         <v>5.120538256262399</v>
@@ -5532,13 +5532,13 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5.288897764652871</v>
+        <v>5.290024598912718</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4280333291601589</v>
+        <v>0.4294870589121006</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3421103565922223</v>
+        <v>0.3421832454412057</v>
       </c>
       <c r="I11" t="n">
         <v>5.325355897311774</v>
@@ -5547,7 +5547,7 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K11" t="n">
-        <v>6.212072171428253</v>
+        <v>6.253239307642481</v>
       </c>
       <c r="L11" t="n">
         <v>5.120538256262399</v>
@@ -5584,13 +5584,13 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>5.249107683373267</v>
+        <v>5.250190011776325</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4625244123311277</v>
+        <v>0.4638677854799723</v>
       </c>
       <c r="H12" t="n">
-        <v>0.32124017332439</v>
+        <v>0.3213064107469701</v>
       </c>
       <c r="I12" t="n">
         <v>5.319232812252986</v>
@@ -5599,7 +5599,7 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K12" t="n">
-        <v>6.260560764738356</v>
+        <v>6.28104364762528</v>
       </c>
       <c r="L12" t="n">
         <v>5.073541154565094</v>
@@ -5636,13 +5636,13 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5.398625870456716</v>
+        <v>5.398708255370416</v>
       </c>
       <c r="G13" t="n">
-        <v>0.4858351601709551</v>
+        <v>0.4859180863416717</v>
       </c>
       <c r="H13" t="n">
-        <v>0.4308572501359106</v>
+        <v>0.4308638251678207</v>
       </c>
       <c r="I13" t="n">
         <v>5.41242710321831</v>
@@ -5688,25 +5688,25 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.6348598052287474</v>
+        <v>0.6403084532179886</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1004679970112869</v>
+        <v>0.09018021305454046</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0353793537493813</v>
+        <v>0.03568299503062096</v>
       </c>
       <c r="I14" t="n">
-        <v>0.6412132427407367</v>
+        <v>0.6430287018168168</v>
       </c>
       <c r="J14" t="n">
-        <v>0.156422771922106</v>
+        <v>0.2730116338200628</v>
       </c>
       <c r="K14" t="n">
         <v>0.8384161921126927</v>
       </c>
       <c r="L14" t="n">
-        <v>0.5860518706266067</v>
+        <v>0.5900421794522246</v>
       </c>
       <c r="M14" t="n">
         <v>0.6929248252164906</v>
@@ -5740,28 +5740,28 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.6314702135540345</v>
+        <v>0.641757298137193</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1060948676036334</v>
+        <v>0.0910953150467934</v>
       </c>
       <c r="H15" t="n">
-        <v>0.03465643034814517</v>
+        <v>0.03522100746150603</v>
       </c>
       <c r="I15" t="n">
-        <v>0.6467984573920755</v>
+        <v>0.6503073688760883</v>
       </c>
       <c r="J15" t="n">
-        <v>0.2131328554039283</v>
+        <v>0.3021365573863949</v>
       </c>
       <c r="K15" t="n">
         <v>0.8208645592673214</v>
       </c>
       <c r="L15" t="n">
-        <v>0.5803096686305257</v>
+        <v>0.5944609730187277</v>
       </c>
       <c r="M15" t="n">
-        <v>0.7078661884691282</v>
+        <v>0.7098636773038356</v>
       </c>
       <c r="N15" t="n">
         <v>332</v>
@@ -5792,25 +5792,25 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.63556144659021</v>
+        <v>0.6399953807246386</v>
       </c>
       <c r="G16" t="n">
-        <v>0.09583282870288122</v>
+        <v>0.08473722631626719</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0391903976944846</v>
+        <v>0.03946380578588422</v>
       </c>
       <c r="I16" t="n">
         <v>0.6471286117195751</v>
       </c>
       <c r="J16" t="n">
-        <v>0.161889743090812</v>
+        <v>0.3184775009384665</v>
       </c>
       <c r="K16" t="n">
         <v>0.8365364011365466</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5924498628907839</v>
+        <v>0.5938764228554572</v>
       </c>
       <c r="M16" t="n">
         <v>0.6981090076183591</v>
@@ -5844,16 +5844,16 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.6261108341379004</v>
+        <v>0.6338811842626941</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1123522439950276</v>
+        <v>0.09753698916333917</v>
       </c>
       <c r="H17" t="n">
-        <v>0.04049974309670352</v>
+        <v>0.04100236526304712</v>
       </c>
       <c r="I17" t="n">
-        <v>0.6490243482647209</v>
+        <v>0.650456303841751</v>
       </c>
       <c r="J17" t="n">
         <v>0.1339871348603871</v>
@@ -5862,10 +5862,10 @@
         <v>0.8061450571977067</v>
       </c>
       <c r="L17" t="n">
-        <v>0.5873476299794895</v>
+        <v>0.5950702466772373</v>
       </c>
       <c r="M17" t="n">
-        <v>0.7039583321258509</v>
+        <v>0.7044900054690548</v>
       </c>
       <c r="N17" t="n">
         <v>239</v>
@@ -5896,28 +5896,28 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.6380304227111452</v>
+        <v>0.6483191854702102</v>
       </c>
       <c r="G18" t="n">
-        <v>0.10294961464393</v>
+        <v>0.08556328058419327</v>
       </c>
       <c r="H18" t="n">
-        <v>0.03904682775458833</v>
+        <v>0.03967648980981436</v>
       </c>
       <c r="I18" t="n">
-        <v>0.6490636564880875</v>
+        <v>0.6515669933999588</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1678435022768646</v>
+        <v>0.3044880769345374</v>
       </c>
       <c r="K18" t="n">
         <v>0.8464523100575919</v>
       </c>
       <c r="L18" t="n">
-        <v>0.5958957988655578</v>
+        <v>0.6057922703803232</v>
       </c>
       <c r="M18" t="n">
-        <v>0.7031610020774126</v>
+        <v>0.7038699287763027</v>
       </c>
       <c r="N18" t="n">
         <v>267</v>
@@ -5948,25 +5948,25 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.6216704326949321</v>
+        <v>0.6227783887708739</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1018076818094732</v>
+        <v>0.09982168892465051</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04961470187951369</v>
+        <v>0.04970312640079123</v>
       </c>
       <c r="I19" t="n">
         <v>0.6333707498663612</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2986005407936297</v>
+        <v>0.3141289514274292</v>
       </c>
       <c r="K19" t="n">
         <v>0.8037858772710206</v>
       </c>
       <c r="L19" t="n">
-        <v>0.5506551939752504</v>
+        <v>0.5610111520498331</v>
       </c>
       <c r="M19" t="n">
         <v>0.6983241065638591</v>
@@ -6403,13 +6403,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.822373116997091</v>
+        <v>1.818662280319711</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3130114696284749</v>
+        <v>0.3078972528397924</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1699371694007676</v>
+        <v>0.1695911320963424</v>
       </c>
       <c r="I2" t="n">
         <v>1.859647236647386</v>
@@ -6418,7 +6418,7 @@
         <v>0.5332906831698536</v>
       </c>
       <c r="K2" t="n">
-        <v>2.451033314752549</v>
+        <v>2.334216937784582</v>
       </c>
       <c r="L2" t="n">
         <v>1.72539489471321</v>
@@ -6455,13 +6455,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.829805332361889</v>
+        <v>1.827811730738236</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2192194546583466</v>
+        <v>0.216980283818827</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2071846554788686</v>
+        <v>0.206958924545499</v>
       </c>
       <c r="I3" t="n">
         <v>1.844157881901027</v>
@@ -6470,7 +6470,7 @@
         <v>0.8700650914891171</v>
       </c>
       <c r="K3" t="n">
-        <v>2.179300960707391</v>
+        <v>2.168069560459498</v>
       </c>
       <c r="L3" t="n">
         <v>1.759816627840232</v>
@@ -6507,13 +6507,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.743424324450679</v>
+        <v>1.740500923226461</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4051843742626012</v>
+        <v>0.3991216055654396</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2441282359538272</v>
+        <v>0.2437188779026377</v>
       </c>
       <c r="I4" t="n">
         <v>1.823652976929057</v>
@@ -6522,13 +6522,13 @@
         <v>0.6020599913279624</v>
       </c>
       <c r="K4" t="n">
-        <v>2.774353943537956</v>
+        <v>2.653413355357386</v>
       </c>
       <c r="L4" t="n">
         <v>1.629985312041806</v>
       </c>
       <c r="M4" t="n">
-        <v>1.994297699106874</v>
+        <v>1.982933520664277</v>
       </c>
       <c r="N4" t="n">
         <v>51</v>
@@ -6559,13 +6559,13 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.821405140602453</v>
+        <v>1.819003605221848</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2196023331868521</v>
+        <v>0.2155098278375565</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2062335210577065</v>
+        <v>0.2059616007218921</v>
       </c>
       <c r="I5" t="n">
         <v>1.848492476877474</v>
@@ -6574,7 +6574,7 @@
         <v>0.7335353824154486</v>
       </c>
       <c r="K5" t="n">
-        <v>2.266728247443086</v>
+        <v>2.237824351104606</v>
       </c>
       <c r="L5" t="n">
         <v>1.725719470475822</v>
@@ -6611,13 +6611,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.266107740095332</v>
+        <v>5.26744148979243</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5897947276321511</v>
+        <v>0.5912883218144948</v>
       </c>
       <c r="H6" t="n">
-        <v>0.491067078835043</v>
+        <v>0.4911914516355963</v>
       </c>
       <c r="I6" t="n">
         <v>5.375348754231917</v>
@@ -6626,7 +6626,7 @@
         <v>2.626385892975756</v>
       </c>
       <c r="K6" t="n">
-        <v>6.205254221641784</v>
+        <v>6.248185116978424</v>
       </c>
       <c r="L6" t="n">
         <v>5.075847164636073</v>
@@ -6663,13 +6663,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.288228068631542</v>
+        <v>5.288505644737421</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4098164857979428</v>
+        <v>0.410092141870719</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5987739193430326</v>
+        <v>0.598805348648024</v>
       </c>
       <c r="I7" t="n">
         <v>5.344753375871109</v>
@@ -6715,13 +6715,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.112515964108585</v>
+        <v>5.112867545578865</v>
       </c>
       <c r="G8" t="n">
-        <v>0.7435710887414629</v>
+        <v>0.7441926011007691</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7158954283816511</v>
+        <v>0.7159446596347258</v>
       </c>
       <c r="I8" t="n">
         <v>5.253751749568488</v>
@@ -6730,13 +6730,13 @@
         <v>2.927415888639737</v>
       </c>
       <c r="K8" t="n">
-        <v>6.571213889318972</v>
+        <v>6.58652356783955</v>
       </c>
       <c r="L8" t="n">
         <v>4.923648462543759</v>
       </c>
       <c r="M8" t="n">
-        <v>5.546238645632577</v>
+        <v>5.547549133864441</v>
       </c>
       <c r="N8" t="n">
         <v>51</v>
@@ -6767,13 +6767,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.26532681535572</v>
+        <v>5.265706644069445</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4125355189639318</v>
+        <v>0.4130785813277644</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5961808630292983</v>
+        <v>0.5962238701622443</v>
       </c>
       <c r="I9" t="n">
         <v>5.341969634498135</v>
@@ -6782,7 +6782,7 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K9" t="n">
-        <v>5.928283610170964</v>
+        <v>5.929581950396245</v>
       </c>
       <c r="L9" t="n">
         <v>5.096178232139799</v>
@@ -6819,25 +6819,25 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.6308633266285653</v>
+        <v>0.6378263869444131</v>
       </c>
       <c r="G10" t="n">
-        <v>0.09913790864469917</v>
+        <v>0.08461099380455878</v>
       </c>
       <c r="H10" t="n">
-        <v>0.05882830854236167</v>
+        <v>0.05947761726482121</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6351090413952435</v>
+        <v>0.638784367416537</v>
       </c>
       <c r="J10" t="n">
-        <v>0.221093604331315</v>
+        <v>0.3270060910884306</v>
       </c>
       <c r="K10" t="n">
         <v>0.8384161921126927</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5860250735164199</v>
+        <v>0.5990230980363649</v>
       </c>
       <c r="M10" t="n">
         <v>0.6784910999751808</v>
@@ -6871,25 +6871,25 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.6382148256467512</v>
+        <v>0.6430963362524357</v>
       </c>
       <c r="G11" t="n">
-        <v>0.08989831622282955</v>
+        <v>0.08403073127623803</v>
       </c>
       <c r="H11" t="n">
-        <v>0.07226359899304137</v>
+        <v>0.07281632122811635</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6437961551684073</v>
+        <v>0.6440873362900528</v>
       </c>
       <c r="J11" t="n">
-        <v>0.4459329127261892</v>
+        <v>0.4528673357440133</v>
       </c>
       <c r="K11" t="n">
         <v>0.8001063651376856</v>
       </c>
       <c r="L11" t="n">
-        <v>0.5828270259492356</v>
+        <v>0.5896497831368773</v>
       </c>
       <c r="M11" t="n">
         <v>0.7068337840769636</v>
@@ -6923,25 +6923,25 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.6417965623255535</v>
+        <v>0.6455067645450334</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1130012395308367</v>
+        <v>0.1028237903509629</v>
       </c>
       <c r="H12" t="n">
-        <v>0.08986949442221139</v>
+        <v>0.09038902664977681</v>
       </c>
       <c r="I12" t="n">
         <v>0.6396973093069322</v>
       </c>
       <c r="J12" t="n">
-        <v>0.156422771922106</v>
+        <v>0.2730116338200628</v>
       </c>
       <c r="K12" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5901590659870052</v>
+        <v>0.5947101006496768</v>
       </c>
       <c r="M12" t="n">
         <v>0.7279574808904055</v>
@@ -6975,25 +6975,25 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.6328614569528442</v>
+        <v>0.6377811310012583</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1033332570131696</v>
+        <v>0.09488164701269411</v>
       </c>
       <c r="H13" t="n">
-        <v>0.07165744935029941</v>
+        <v>0.07221449274434906</v>
       </c>
       <c r="I13" t="n">
         <v>0.6533142429574215</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3011425009798275</v>
+        <v>0.3363613402899823</v>
       </c>
       <c r="K13" t="n">
         <v>0.8354377826444299</v>
       </c>
       <c r="L13" t="n">
-        <v>0.5864452265754659</v>
+        <v>0.5894019161070462</v>
       </c>
       <c r="M13" t="n">
         <v>0.6909321454135275</v>
@@ -7326,13 +7326,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.839293707625931</v>
+        <v>1.835850864016455</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1986058827488095</v>
+        <v>0.1952627429434063</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1665218280112236</v>
+        <v>0.166210127596532</v>
       </c>
       <c r="I2" t="n">
         <v>1.833091327047386</v>
@@ -7347,7 +7347,7 @@
         <v>1.764943140035772</v>
       </c>
       <c r="M2" t="n">
-        <v>1.947807132997508</v>
+        <v>1.940680200614224</v>
       </c>
       <c r="N2" t="n">
         <v>122</v>
@@ -7378,13 +7378,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.844209929282749</v>
+        <v>1.841121694748109</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1587664648962644</v>
+        <v>0.1545197241346241</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2101672266536502</v>
+        <v>0.2098152896658401</v>
       </c>
       <c r="I3" t="n">
         <v>1.824307600928442</v>
@@ -7393,7 +7393,7 @@
         <v>1.47212508281708</v>
       </c>
       <c r="K3" t="n">
-        <v>2.206475217546849</v>
+        <v>2.185698900524835</v>
       </c>
       <c r="L3" t="n">
         <v>1.758258510508658</v>
@@ -7430,13 +7430,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.758949366836547</v>
+        <v>1.74753751662678</v>
       </c>
       <c r="G4" t="n">
-        <v>0.286551425451853</v>
+        <v>0.2732707267074966</v>
       </c>
       <c r="H4" t="n">
-        <v>0.19916179722922</v>
+        <v>0.1978696596382582</v>
       </c>
       <c r="I4" t="n">
         <v>1.81156671351466</v>
@@ -7445,13 +7445,13 @@
         <v>0.8343206788338349</v>
       </c>
       <c r="K4" t="n">
-        <v>2.352092404829444</v>
+        <v>2.219427636816201</v>
       </c>
       <c r="L4" t="n">
-        <v>1.698404975497838</v>
+        <v>1.696508440195641</v>
       </c>
       <c r="M4" t="n">
-        <v>1.904873011886297</v>
+        <v>1.895178175327752</v>
       </c>
       <c r="N4" t="n">
         <v>78</v>
@@ -7482,13 +7482,13 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.729912635383377</v>
+        <v>1.729178783508723</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2646739857030106</v>
+        <v>0.2641044189841782</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2332613721697794</v>
+        <v>0.2331624196031875</v>
       </c>
       <c r="I5" t="n">
         <v>1.762674775347484</v>
@@ -7503,7 +7503,7 @@
         <v>1.634881621807715</v>
       </c>
       <c r="M5" t="n">
-        <v>1.928647525035563</v>
+        <v>1.925372075792436</v>
       </c>
       <c r="N5" t="n">
         <v>55</v>
@@ -7534,13 +7534,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.304663209088449</v>
+        <v>5.305572916438691</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3677677525162041</v>
+        <v>0.3684159021384901</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4802616411391232</v>
+        <v>0.4803440021727577</v>
       </c>
       <c r="I6" t="n">
         <v>5.311231254620168</v>
@@ -7586,13 +7586,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.311083170982762</v>
+        <v>5.311694682677721</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2762442070980988</v>
+        <v>0.2770078076907949</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6052540997902774</v>
+        <v>0.6053237880155466</v>
       </c>
       <c r="I7" t="n">
         <v>5.29383884586571</v>
@@ -7638,13 +7638,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.126758849452423</v>
+        <v>5.130311239902221</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5156596350331015</v>
+        <v>0.519365230425466</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5804911304832548</v>
+        <v>0.580893359495517</v>
       </c>
       <c r="I8" t="n">
         <v>5.266811605822859</v>
@@ -7653,7 +7653,7 @@
         <v>3.404537143359399</v>
       </c>
       <c r="K8" t="n">
-        <v>5.992435102775991</v>
+        <v>6.051920113474019</v>
       </c>
       <c r="L8" t="n">
         <v>5.077402309227036</v>
@@ -7690,13 +7690,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.084976827140425</v>
+        <v>5.085106809718418</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5028412107137312</v>
+        <v>0.5029001355274928</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6856581354973695</v>
+        <v>0.6856756623446106</v>
       </c>
       <c r="I9" t="n">
         <v>5.177835890948631</v>
@@ -7742,16 +7742,16 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.6374305796343332</v>
+        <v>0.6454101172883621</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1015604392982377</v>
+        <v>0.09171152166159474</v>
       </c>
       <c r="H10" t="n">
-        <v>0.05771025307750938</v>
+        <v>0.05843268647209125</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6476919760863287</v>
+        <v>0.6509944478642216</v>
       </c>
       <c r="J10" t="n">
         <v>0.3021365573863949</v>
@@ -7760,10 +7760,10 @@
         <v>0.8073389888685292</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5878221414198488</v>
+        <v>0.5931548866302427</v>
       </c>
       <c r="M10" t="n">
-        <v>0.7087933998054654</v>
+        <v>0.7105718979539957</v>
       </c>
       <c r="N10" t="n">
         <v>122</v>
@@ -7794,28 +7794,28 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.6316159321451285</v>
+        <v>0.6390293839998907</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09953426017371157</v>
+        <v>0.09221633897943983</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0719793157283504</v>
+        <v>0.07282415697527489</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6324835971220547</v>
+        <v>0.6327956768832609</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3420900372824928</v>
+        <v>0.3786667170172284</v>
       </c>
       <c r="K11" t="n">
         <v>0.7831728970924439</v>
       </c>
       <c r="L11" t="n">
-        <v>0.5725275100098002</v>
+        <v>0.579828396427419</v>
       </c>
       <c r="M11" t="n">
-        <v>0.7138950869189147</v>
+        <v>0.7143806831586477</v>
       </c>
       <c r="N11" t="n">
         <v>77</v>
@@ -7846,25 +7846,25 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.6191227555306096</v>
+        <v>0.6421335165485201</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1211680174434936</v>
+        <v>0.08408331653066552</v>
       </c>
       <c r="H12" t="n">
-        <v>0.07010184774036282</v>
+        <v>0.07270730336423981</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6513119486635524</v>
+        <v>0.6520993625638969</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2131328554039283</v>
+        <v>0.3538969080190041</v>
       </c>
       <c r="K12" t="n">
         <v>0.8085181266789708</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5791943975649724</v>
+        <v>0.6004830690146081</v>
       </c>
       <c r="M12" t="n">
         <v>0.6984921899424941</v>
@@ -7898,13 +7898,13 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.6355559723270608</v>
+        <v>0.636940214792577</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1003175464349812</v>
+        <v>0.09715655559209509</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0856983498261193</v>
+        <v>0.08588500104209265</v>
       </c>
       <c r="I13" t="n">
         <v>0.6460199816628208</v>
@@ -8249,13 +8249,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.82605734386849</v>
+        <v>1.825266844372152</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2260096414970699</v>
+        <v>0.2237069441760299</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1733216928635348</v>
+        <v>0.173246661971776</v>
       </c>
       <c r="I2" t="n">
         <v>1.803158942439264</v>
@@ -8264,7 +8264,7 @@
         <v>0.8700650914891171</v>
       </c>
       <c r="K2" t="n">
-        <v>2.52453914055526</v>
+        <v>2.50802428552143</v>
       </c>
       <c r="L2" t="n">
         <v>1.702724950076516</v>
@@ -8301,13 +8301,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.851539390937015</v>
+        <v>1.844993214607022</v>
       </c>
       <c r="G3" t="n">
-        <v>0.258772986376438</v>
+        <v>0.247560317622085</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2123861340810341</v>
+        <v>0.2116352361576384</v>
       </c>
       <c r="I3" t="n">
         <v>1.850641869783991</v>
@@ -8316,13 +8316,13 @@
         <v>0.8700650914891171</v>
       </c>
       <c r="K3" t="n">
-        <v>2.774310952382516</v>
+        <v>2.616753228591421</v>
       </c>
       <c r="L3" t="n">
         <v>1.72695708534711</v>
       </c>
       <c r="M3" t="n">
-        <v>1.984158528435025</v>
+        <v>1.9779733892752</v>
       </c>
       <c r="N3" t="n">
         <v>76</v>
@@ -8353,13 +8353,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.865250288095267</v>
+        <v>1.864015229830585</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1600138436519009</v>
+        <v>0.158927725342847</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2139588818478262</v>
+        <v>0.2138172109487438</v>
       </c>
       <c r="I4" t="n">
         <v>1.884665736473232</v>
@@ -8374,7 +8374,7 @@
         <v>1.787591822460185</v>
       </c>
       <c r="M4" t="n">
-        <v>1.956254629974546</v>
+        <v>1.955317561999014</v>
       </c>
       <c r="N4" t="n">
         <v>76</v>
@@ -8405,13 +8405,13 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>5.288579172123786</v>
+        <v>5.288922689665581</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4101541538313361</v>
+        <v>0.4109582632791246</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5019697207391424</v>
+        <v>0.5020023259812899</v>
       </c>
       <c r="I5" t="n">
         <v>5.274745903956688</v>
@@ -8457,13 +8457,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.320154011556962</v>
+        <v>5.321401522556875</v>
       </c>
       <c r="G6" t="n">
-        <v>0.454195088867999</v>
+        <v>0.4557323102451877</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6102635184328767</v>
+        <v>0.610406617758655</v>
       </c>
       <c r="I6" t="n">
         <v>5.324049089510432</v>
@@ -8472,7 +8472,7 @@
         <v>3.471483932990012</v>
       </c>
       <c r="K6" t="n">
-        <v>6.586047263249251</v>
+        <v>6.610643094681172</v>
       </c>
       <c r="L6" t="n">
         <v>5.140142972694157</v>
@@ -8509,16 +8509,16 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.346395491075349</v>
+        <v>5.346931761644491</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3052277919736267</v>
+        <v>0.305311257489175</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6132736225736567</v>
+        <v>0.6133351370267432</v>
       </c>
       <c r="I7" t="n">
-        <v>5.376894287827102</v>
+        <v>5.379958144524353</v>
       </c>
       <c r="J7" t="n">
         <v>3.626385892975756</v>
@@ -8561,19 +8561,19 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.6503281871288471</v>
+        <v>0.6513404168330644</v>
       </c>
       <c r="G8" t="n">
-        <v>0.08671493688544056</v>
+        <v>0.08229485921932</v>
       </c>
       <c r="H8" t="n">
-        <v>0.06172641986765726</v>
+        <v>0.06182249645938687</v>
       </c>
       <c r="I8" t="n">
         <v>0.6608814417664505</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2256501675611327</v>
+        <v>0.3380076647292516</v>
       </c>
       <c r="K8" t="n">
         <v>0.8365364011365466</v>
@@ -8613,25 +8613,25 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.6297469581401088</v>
+        <v>0.6416437229132438</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1152284214958619</v>
+        <v>0.0925932389968107</v>
       </c>
       <c r="H9" t="n">
-        <v>0.07223693027723349</v>
+        <v>0.0736015827877906</v>
       </c>
       <c r="I9" t="n">
         <v>0.648879701617272</v>
       </c>
       <c r="J9" t="n">
-        <v>0.161889743090812</v>
+        <v>0.3184775009384665</v>
       </c>
       <c r="K9" t="n">
         <v>0.833577575558071</v>
       </c>
       <c r="L9" t="n">
-        <v>0.5870982638812882</v>
+        <v>0.5922716991639744</v>
       </c>
       <c r="M9" t="n">
         <v>0.7020301430158876</v>
@@ -8665,19 +8665,19 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.6198087218851963</v>
+        <v>0.6217773147460961</v>
       </c>
       <c r="G10" t="n">
-        <v>0.08319142446440181</v>
+        <v>0.07655400143290453</v>
       </c>
       <c r="H10" t="n">
-        <v>0.07109693639533361</v>
+        <v>0.07132274948327144</v>
       </c>
       <c r="I10" t="n">
         <v>0.6242643208696557</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2766829708071901</v>
+        <v>0.4262960282355666</v>
       </c>
       <c r="K10" t="n">
         <v>0.7565567975613332</v>
@@ -8964,13 +8964,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.861739111028721</v>
+        <v>1.856461037080761</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2107108369016559</v>
+        <v>0.2008250629856769</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2209477829311016</v>
+        <v>0.2203213907958985</v>
       </c>
       <c r="I2" t="n">
         <v>1.836497653201626</v>
@@ -8979,13 +8979,13 @@
         <v>0.7335353824154486</v>
       </c>
       <c r="K2" t="n">
-        <v>2.533621135627763</v>
+        <v>2.377796100002772</v>
       </c>
       <c r="L2" t="n">
         <v>1.762292109281748</v>
       </c>
       <c r="M2" t="n">
-        <v>1.978616579180455</v>
+        <v>1.965697877474259</v>
       </c>
       <c r="N2" t="n">
         <v>71</v>
@@ -9016,13 +9016,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.860256990611487</v>
+        <v>1.853832882865031</v>
       </c>
       <c r="G3" t="n">
-        <v>0.215193178713189</v>
+        <v>0.2026763993889318</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2401581448101406</v>
+        <v>0.2393287960662649</v>
       </c>
       <c r="I3" t="n">
         <v>1.837117438061018</v>
@@ -9068,13 +9068,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.850303775460095</v>
+        <v>1.846893891337996</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2244176244999545</v>
+        <v>0.2201489369992825</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2122443992653244</v>
+        <v>0.2118532587311819</v>
       </c>
       <c r="I4" t="n">
         <v>1.874186838451467</v>
@@ -9172,13 +9172,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.329947493125379</v>
+        <v>5.331660051827842</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3819043493150406</v>
+        <v>0.3844415918022907</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6325483923977508</v>
+        <v>0.6327516357234172</v>
       </c>
       <c r="I6" t="n">
         <v>5.309432931214605</v>
@@ -9187,13 +9187,13 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K6" t="n">
-        <v>6.212072171428253</v>
+        <v>6.253239307642481</v>
       </c>
       <c r="L6" t="n">
         <v>5.132857204574069</v>
       </c>
       <c r="M6" t="n">
-        <v>5.563440015474354</v>
+        <v>5.573708937822836</v>
       </c>
       <c r="N6" t="n">
         <v>71</v>
@@ -9224,13 +9224,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.341440417148941</v>
+        <v>5.342593280034484</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3360389622706493</v>
+        <v>0.3381783433037336</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6895769926792348</v>
+        <v>0.6897258266377737</v>
       </c>
       <c r="I7" t="n">
         <v>5.329574218251185</v>
@@ -9239,7 +9239,7 @@
         <v>4.560884344219324</v>
       </c>
       <c r="K7" t="n">
-        <v>6.066192104369086</v>
+        <v>6.093993998559389</v>
       </c>
       <c r="L7" t="n">
         <v>5.078173328522412</v>
@@ -9276,13 +9276,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.311334038516857</v>
+        <v>5.312367590452334</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4059820677571992</v>
+        <v>0.4068319233920745</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6092517981390195</v>
+        <v>0.609370354676905</v>
       </c>
       <c r="I8" t="n">
         <v>5.377271435925309</v>
@@ -9380,28 +9380,28 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.6138223711720885</v>
+        <v>0.6232851781866745</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1106988649379014</v>
+        <v>0.09342118969876029</v>
       </c>
       <c r="H10" t="n">
-        <v>0.07284731314960941</v>
+        <v>0.07397034172960329</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6307714539166999</v>
+        <v>0.6356587283462203</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2073117298810935</v>
+        <v>0.2925441460429838</v>
       </c>
       <c r="K10" t="n">
         <v>0.7613656943893731</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5825025337862184</v>
+        <v>0.5828532116235918</v>
       </c>
       <c r="M10" t="n">
-        <v>0.6837465310099287</v>
+        <v>0.6858417740941932</v>
       </c>
       <c r="N10" t="n">
         <v>71</v>
@@ -9432,16 +9432,16 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.6415969606119817</v>
+        <v>0.6535073299466521</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1272103085246641</v>
+        <v>0.1054627021994252</v>
       </c>
       <c r="H11" t="n">
-        <v>0.08282981144758336</v>
+        <v>0.08436743351692863</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6753983256456151</v>
+        <v>0.6771535447492846</v>
       </c>
       <c r="J11" t="n">
         <v>0.1339871348603871</v>
@@ -9450,7 +9450,7 @@
         <v>0.7875377343848247</v>
       </c>
       <c r="L11" t="n">
-        <v>0.6299003949672075</v>
+        <v>0.6318355433510419</v>
       </c>
       <c r="M11" t="n">
         <v>0.7134443933618393</v>
@@ -9484,25 +9484,25 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.617238965590627</v>
+        <v>0.6234314948236519</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1054286272742007</v>
+        <v>0.09283175848156104</v>
       </c>
       <c r="H12" t="n">
-        <v>0.07080216513224005</v>
+        <v>0.07151249695149471</v>
       </c>
       <c r="I12" t="n">
         <v>0.6319022959418358</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2360578399885129</v>
+        <v>0.3389184823098451</v>
       </c>
       <c r="K12" t="n">
         <v>0.7853981633974483</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5635091918045312</v>
+        <v>0.5735711000400433</v>
       </c>
       <c r="M12" t="n">
         <v>0.6867650603180195</v>
@@ -9887,13 +9887,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.793729265490044</v>
+        <v>1.788238865714853</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3097723470420167</v>
+        <v>0.3016923692067361</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1750500521041652</v>
+        <v>0.1745142439500527</v>
       </c>
       <c r="I2" t="n">
         <v>1.837133213530358</v>
@@ -9902,7 +9902,7 @@
         <v>0.8700650914891171</v>
       </c>
       <c r="K2" t="n">
-        <v>2.454990292960388</v>
+        <v>2.378936282253052</v>
       </c>
       <c r="L2" t="n">
         <v>1.712282156461322</v>
@@ -9939,13 +9939,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.865164908461524</v>
+        <v>1.859078228273727</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2106707980979219</v>
+        <v>0.2027223836013365</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2198117924673883</v>
+        <v>0.2190944703281042</v>
       </c>
       <c r="I3" t="n">
         <v>1.872191235717531</v>
@@ -9954,13 +9954,13 @@
         <v>0.7335353824154486</v>
       </c>
       <c r="K3" t="n">
-        <v>2.430230651837887</v>
+        <v>2.349272620365455</v>
       </c>
       <c r="L3" t="n">
         <v>1.77473154462517</v>
       </c>
       <c r="M3" t="n">
-        <v>1.962886188184603</v>
+        <v>1.952427051541087</v>
       </c>
       <c r="N3" t="n">
         <v>72</v>
@@ -9991,13 +9991,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>1.785504857924119</v>
+        <v>1.784094550362472</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1521894580504917</v>
+        <v>0.1488421068703992</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2452579542175809</v>
+        <v>0.245064233575572</v>
       </c>
       <c r="I4" t="n">
         <v>1.797460901243169</v>
@@ -10006,7 +10006,7 @@
         <v>1.436380670161797</v>
       </c>
       <c r="K4" t="n">
-        <v>2.179420589519776</v>
+        <v>2.104674288752506</v>
       </c>
       <c r="L4" t="n">
         <v>1.680330934136923</v>
@@ -10043,16 +10043,16 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1.795837616653278</v>
+        <v>1.789053880884682</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2456979670596483</v>
+        <v>0.238380731218867</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2952338855426654</v>
+        <v>0.2941186462521611</v>
       </c>
       <c r="I5" t="n">
-        <v>1.836497653201626</v>
+        <v>1.833415740547789</v>
       </c>
       <c r="J5" t="n">
         <v>0.7953683386006525</v>
@@ -10095,13 +10095,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.205782244922166</v>
+        <v>5.207158367744126</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5651045067024409</v>
+        <v>0.5670332163422873</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5080323272573721</v>
+        <v>0.5081666230936057</v>
       </c>
       <c r="I6" t="n">
         <v>5.29663174604988</v>
@@ -10110,7 +10110,7 @@
         <v>3.471483932990012</v>
       </c>
       <c r="K6" t="n">
-        <v>6.260560764738356</v>
+        <v>6.28104364762528</v>
       </c>
       <c r="L6" t="n">
         <v>5.075092212880835</v>
@@ -10147,13 +10147,13 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>5.349814562953796</v>
+        <v>5.350748239669108</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3916760636671771</v>
+        <v>0.3927420441508138</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6304816925925293</v>
+        <v>0.6305917274486681</v>
       </c>
       <c r="I7" t="n">
         <v>5.37064433000247</v>
@@ -10162,7 +10162,7 @@
         <v>3.103507147695418</v>
       </c>
       <c r="K7" t="n">
-        <v>6.141597197303557</v>
+        <v>6.159012894204647</v>
       </c>
       <c r="L7" t="n">
         <v>5.215590306235367</v>
@@ -10199,13 +10199,13 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.221644300552574</v>
+        <v>5.221808896182855</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2879106867845075</v>
+        <v>0.2882796535161263</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7172480058633595</v>
+        <v>0.7172706148119583</v>
       </c>
       <c r="I8" t="n">
         <v>5.257829661988928</v>
@@ -10214,7 +10214,7 @@
         <v>4.594868841529691</v>
       </c>
       <c r="K8" t="n">
-        <v>5.863174992385049</v>
+        <v>5.871898560789906</v>
       </c>
       <c r="L8" t="n">
         <v>5.022585240071492</v>
@@ -10251,13 +10251,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.215427548158789</v>
+        <v>5.2172799939805</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4392832291749252</v>
+        <v>0.4403749248585409</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8574110072817674</v>
+        <v>0.8577155474988949</v>
       </c>
       <c r="I9" t="n">
         <v>5.339035594602967</v>
@@ -10303,25 +10303,25 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.6295797535170017</v>
+        <v>0.6404914609981889</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1154117024370251</v>
+        <v>0.0967657250097162</v>
       </c>
       <c r="H10" t="n">
-        <v>0.06144069273841615</v>
+        <v>0.06250556635110452</v>
       </c>
       <c r="I10" t="n">
-        <v>0.6443216217014205</v>
+        <v>0.6458796443866489</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2531892856004807</v>
+        <v>0.3044880769345374</v>
       </c>
       <c r="K10" t="n">
         <v>0.8464523100575919</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5761483680386109</v>
+        <v>0.5812927123697004</v>
       </c>
       <c r="M10" t="n">
         <v>0.7027251761545028</v>
@@ -10355,28 +10355,28 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0.6271171298658957</v>
+        <v>0.6410951771173352</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09478569709178633</v>
+        <v>0.07802624108254129</v>
       </c>
       <c r="H11" t="n">
-        <v>0.07390646252106994</v>
+        <v>0.07555379118760976</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6274170471411614</v>
+        <v>0.6342381516643567</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2837460790977951</v>
+        <v>0.4093166263729265</v>
       </c>
       <c r="K11" t="n">
         <v>0.7848238233496453</v>
       </c>
       <c r="L11" t="n">
-        <v>0.5937936334006353</v>
+        <v>0.6048644977578892</v>
       </c>
       <c r="M11" t="n">
-        <v>0.6819150822351339</v>
+        <v>0.6868662601079942</v>
       </c>
       <c r="N11" t="n">
         <v>72</v>
@@ -10407,25 +10407,25 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>0.6677451025206936</v>
+        <v>0.671422796504884</v>
       </c>
       <c r="G12" t="n">
-        <v>0.06499736218331012</v>
+        <v>0.05920908420796121</v>
       </c>
       <c r="H12" t="n">
-        <v>0.09172184385621765</v>
+        <v>0.09222701397591675</v>
       </c>
       <c r="I12" t="n">
         <v>0.6763524690463859</v>
       </c>
       <c r="J12" t="n">
-        <v>0.4743815488499469</v>
+        <v>0.5133981787779858</v>
       </c>
       <c r="K12" t="n">
         <v>0.8164707599066954</v>
       </c>
       <c r="L12" t="n">
-        <v>0.6292426189235606</v>
+        <v>0.6459925863511383</v>
       </c>
       <c r="M12" t="n">
         <v>0.704143029552283</v>
@@ -10459,25 +10459,25 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.6406844583959277</v>
+        <v>0.6514961661764674</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1159376853189024</v>
+        <v>0.09131886403973632</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1053278761425718</v>
+        <v>0.107105309952734</v>
       </c>
       <c r="I13" t="n">
-        <v>0.6508153815551437</v>
+        <v>0.6638675949312507</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1678435022768646</v>
+        <v>0.3917485527260929</v>
       </c>
       <c r="K13" t="n">
         <v>0.8143939788008583</v>
       </c>
       <c r="L13" t="n">
-        <v>0.6058789241179394</v>
+        <v>0.6091718257607061</v>
       </c>
       <c r="M13" t="n">
         <v>0.7251850111984403</v>
@@ -10810,13 +10810,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1.879217475482694</v>
+        <v>1.877856201000336</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3047812384065106</v>
+        <v>0.303234412966798</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2313156809315824</v>
+        <v>0.2311481196259169</v>
       </c>
       <c r="I2" t="n">
         <v>1.868036735559411</v>
@@ -11018,13 +11018,13 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5.365768304632034</v>
+        <v>5.365964280866139</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5526280457721844</v>
+        <v>0.5528130832618453</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6604804208668035</v>
+        <v>0.660504543873656</v>
       </c>
       <c r="I6" t="n">
         <v>5.386127940904656</v>
@@ -11226,25 +11226,25 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.6136642840154694</v>
+        <v>0.6162998764991492</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1131623950218726</v>
+        <v>0.1090474877570272</v>
       </c>
       <c r="H10" t="n">
-        <v>0.07553685168022882</v>
+        <v>0.0758612706886589</v>
       </c>
       <c r="I10" t="n">
         <v>0.6363839579933862</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2986005407936297</v>
+        <v>0.3141289514274292</v>
       </c>
       <c r="K10" t="n">
         <v>0.8001063651376856</v>
       </c>
       <c r="L10" t="n">
-        <v>0.5455443659941593</v>
+        <v>0.5476376034867927</v>
       </c>
       <c r="M10" t="n">
         <v>0.6971427282716451</v>

</xml_diff>